<commit_message>
Added F1 score to analysis
</commit_message>
<xml_diff>
--- a/output/inference/Results.xlsx
+++ b/output/inference/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TP</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -134,6 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,6 +590,15 @@
         <v>0.95477386934673369</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1">
+        <f>2*K9*K10/(K9 + K10)</f>
+        <v>0.97435897435897434</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>